<commit_message>
Zrobiłem instrukcje sterujące estymacją + wczytywanie parametrów z XLS
</commit_message>
<xml_diff>
--- a/Smets_Warne_Wouters_2014/Model_Inputs.xlsx
+++ b/Smets_Warne_Wouters_2014/Model_Inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\DSGE_Routledge\Smets_Warne_Wouters_2014\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEAAF00E-E7CF-4007-A74C-52460F80906F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47432933-2F46-4A9E-BE2A-9FDB84966661}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{66EF218B-DC11-4D6A-BEE5-8BD9D8BBF969}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11295" xr2:uid="{66EF218B-DC11-4D6A-BEE5-8BD9D8BBF969}"/>
   </bookViews>
   <sheets>
     <sheet name="Parametry" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="109">
   <si>
     <t>c_rho_b</t>
   </si>
@@ -159,24 +159,12 @@
     <t>Habit parameter</t>
   </si>
   <si>
-    <t>c_tau</t>
-  </si>
-  <si>
     <t>${\tau}$</t>
   </si>
   <si>
-    <t>Trend growth rate</t>
-  </si>
-  <si>
-    <t>c_beta</t>
-  </si>
-  <si>
     <t>${\beta}$</t>
   </si>
   <si>
-    <t>Discount factor</t>
-  </si>
-  <si>
     <t>c_phi</t>
   </si>
   <si>
@@ -258,15 +246,6 @@
     <t>Probability of wage change</t>
   </si>
   <si>
-    <t>c_eps_w</t>
-  </si>
-  <si>
-    <t>${\varepsilon_w}$</t>
-  </si>
-  <si>
-    <t>Curvature of the wage aggregator function</t>
-  </si>
-  <si>
     <t>c_omega</t>
   </si>
   <si>
@@ -337,6 +316,54 @@
   </si>
   <si>
     <t>Fraction of firms able to adjust employment</t>
+  </si>
+  <si>
+    <t>c_psi_w</t>
+  </si>
+  <si>
+    <t>${\psi^w}$</t>
+  </si>
+  <si>
+    <t>Steady state labor market markup parameter</t>
+  </si>
+  <si>
+    <t>c_e_bar</t>
+  </si>
+  <si>
+    <t>Steady state employment</t>
+  </si>
+  <si>
+    <t>${\bar{e}}$</t>
+  </si>
+  <si>
+    <t>c_beta_bar</t>
+  </si>
+  <si>
+    <t>Steady state discount factor</t>
+  </si>
+  <si>
+    <t>c_tau_bar</t>
+  </si>
+  <si>
+    <t>Steady state average growth rate</t>
+  </si>
+  <si>
+    <t>c_pi_bar</t>
+  </si>
+  <si>
+    <t>Target inflation (steady state)</t>
+  </si>
+  <si>
+    <t>${\bar{\pi}}$</t>
+  </si>
+  <si>
+    <t>c_gy</t>
+  </si>
+  <si>
+    <t>Steady state government spending-output ratio</t>
+  </si>
+  <si>
+    <t>${\frac{\bar{g}}{y}}$</t>
   </si>
 </sst>
 </file>
@@ -344,9 +371,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="#,##0.000"/>
+    <numFmt numFmtId="164" formatCode="#,##0.000"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -366,6 +393,12 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial Unicode MS"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -388,7 +421,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -399,19 +432,23 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -746,11 +783,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BE39027-846B-4168-A1BF-4076619A79DB}">
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -775,351 +810,410 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="3" t="s">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D2" s="5">
-        <v>0.63531800000000005</v>
-      </c>
-      <c r="F2" s="3"/>
+        <v>53</v>
+      </c>
+      <c r="D2" s="6">
+        <v>0.22679099999999999</v>
+      </c>
+      <c r="F2" s="9"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="3" t="s">
-        <v>40</v>
+        <v>99</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>41</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D3" s="5">
-        <v>4.6308819999999997</v>
-      </c>
-      <c r="F3" s="3"/>
+        <v>100</v>
+      </c>
+      <c r="D3" s="6">
+        <v>0.26856000000000002</v>
+      </c>
+      <c r="E3" s="5"/>
+      <c r="G3" s="9"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="3" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D4" s="5">
-        <v>1.4906619999999999</v>
-      </c>
-      <c r="F4" s="3"/>
+        <v>47</v>
+      </c>
+      <c r="D4" s="6">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E4" s="5"/>
+      <c r="G4" s="9"/>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="3" t="s">
-        <v>46</v>
+      <c r="A5" t="s">
+        <v>96</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>47</v>
+        <v>98</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D5" s="5">
-        <v>0.22679099999999999</v>
-      </c>
-      <c r="F5" s="3"/>
+        <v>97</v>
+      </c>
+      <c r="D5" s="6">
+        <v>0.22636700000000001</v>
+      </c>
+      <c r="E5" s="5"/>
+      <c r="G5" s="9"/>
       <c r="H5" s="2"/>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="3" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D6" s="5">
-        <v>0.25043199999999999</v>
-      </c>
-      <c r="F6" s="3"/>
+        <v>62</v>
+      </c>
+      <c r="D6" s="6">
+        <v>10</v>
+      </c>
+      <c r="E6" s="5"/>
+      <c r="G6" s="9"/>
       <c r="H6" s="2"/>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="3" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D7" s="5">
-        <v>0.84280200000000005</v>
-      </c>
-      <c r="F7" s="3"/>
+        <v>56</v>
+      </c>
+      <c r="D7" s="6">
+        <v>0.25043199999999999</v>
+      </c>
+      <c r="E7" s="5"/>
+      <c r="G7" s="9"/>
       <c r="H7" s="2"/>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="3" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D8" s="5">
+        <v>65</v>
+      </c>
+      <c r="D8" s="6">
         <v>0.25178099999999998</v>
       </c>
-      <c r="F8" s="3"/>
+      <c r="E8" s="5"/>
+      <c r="G8" s="9"/>
       <c r="H8" s="2"/>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="3" t="s">
-        <v>58</v>
+      <c r="A9" t="s">
+        <v>106</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>59</v>
+        <v>108</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D9" s="5">
-        <v>0.69631100000000001</v>
-      </c>
-      <c r="F9" s="3"/>
+        <v>107</v>
+      </c>
+      <c r="D9" s="6">
+        <v>0.18</v>
+      </c>
+      <c r="E9" s="5"/>
+      <c r="G9" s="9"/>
       <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="3" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>62</v>
+        <v>38</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>63</v>
+        <v>39</v>
       </c>
       <c r="D10" s="5">
-        <v>1.5002359999999999</v>
-      </c>
-      <c r="F10" s="3"/>
+        <v>0.63531800000000005</v>
+      </c>
+      <c r="E10" s="5"/>
+      <c r="G10" s="9"/>
       <c r="H10" s="2"/>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="3" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="D11" s="5">
+        <v>71</v>
+      </c>
+      <c r="D11" s="6">
         <v>5.3859640000000004</v>
       </c>
-      <c r="F11" s="3"/>
+      <c r="E11" s="5"/>
+      <c r="G11" s="9"/>
       <c r="H11" s="2"/>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="3" t="s">
-        <v>67</v>
+        <v>42</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>68</v>
+        <v>43</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>69</v>
+        <v>44</v>
       </c>
       <c r="D12" s="5">
-        <v>8.5280999999999996E-2</v>
-      </c>
-      <c r="F12" s="3"/>
+        <v>4.6308819999999997</v>
+      </c>
+      <c r="E12" s="5"/>
+      <c r="G12" s="9"/>
       <c r="H12" s="2"/>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="3" t="s">
-        <v>70</v>
+      <c r="A13" t="s">
+        <v>103</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>71</v>
+        <v>105</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D13" s="5">
-        <v>0.47281000000000001</v>
-      </c>
-      <c r="F13" s="3"/>
+        <v>104</v>
+      </c>
+      <c r="D13" s="6">
+        <v>0.56137000000000004</v>
+      </c>
+      <c r="E13" s="5"/>
+      <c r="G13" s="9"/>
       <c r="H13" s="2"/>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="3" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D14" s="5">
-        <v>0.85638300000000001</v>
-      </c>
-      <c r="F14" s="3"/>
+        <v>77</v>
+      </c>
+      <c r="D14" s="6">
+        <v>0.47281000000000001</v>
+      </c>
+      <c r="E14" s="5"/>
+      <c r="G14" s="9"/>
       <c r="H14" s="2"/>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="3" t="s">
-        <v>76</v>
+        <v>48</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>77</v>
+        <v>49</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>78</v>
+        <v>50</v>
       </c>
       <c r="D15" s="5">
-        <v>1.287264</v>
-      </c>
-      <c r="F15" s="3"/>
+        <v>1.4906619999999999</v>
+      </c>
+      <c r="E15" s="5"/>
+      <c r="G15" s="9"/>
       <c r="H15" s="2"/>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="3" t="s">
-        <v>79</v>
+        <v>93</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>80</v>
+        <v>94</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="D16" s="5">
-        <v>0.19212399999999999</v>
-      </c>
-      <c r="F16" s="3"/>
+        <v>95</v>
+      </c>
+      <c r="D16" s="6">
+        <v>1.5002359999999999</v>
+      </c>
+      <c r="E16" s="5"/>
+      <c r="G16" s="9"/>
       <c r="H16" s="2"/>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="3" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="D17" s="5">
+        <v>89</v>
+      </c>
+      <c r="D17" s="6">
         <v>1.6608000000000001E-2</v>
       </c>
-      <c r="F17" s="3"/>
+      <c r="E17" s="5"/>
+      <c r="G17" s="9"/>
       <c r="H17" s="2"/>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="3" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="D18" s="5">
-        <v>0.70556700000000006</v>
-      </c>
-      <c r="F18" s="3"/>
+        <v>80</v>
+      </c>
+      <c r="D18" s="6">
+        <v>0.85638300000000001</v>
+      </c>
+      <c r="E18" s="5"/>
+      <c r="G18" s="9"/>
       <c r="H18" s="2"/>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="3" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="D19" s="5">
-        <v>0.56137000000000004</v>
-      </c>
-      <c r="F19" s="3"/>
+        <v>83</v>
+      </c>
+      <c r="D19" s="6">
+        <v>1.287264</v>
+      </c>
+      <c r="G19" s="9"/>
       <c r="H19" s="2"/>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="3" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D20" s="5">
-        <v>0.26856000000000002</v>
-      </c>
-      <c r="F20" s="3"/>
+        <v>86</v>
+      </c>
+      <c r="D20" s="6">
+        <v>0.19212399999999999</v>
+      </c>
+      <c r="G20" s="9"/>
       <c r="H20" s="2"/>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="3" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>95</v>
+        <v>40</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="D21" s="5">
-        <v>0.22636700000000001</v>
-      </c>
-      <c r="F21" s="3"/>
+        <v>102</v>
+      </c>
+      <c r="D21" s="6">
+        <v>0.13084799999999999</v>
+      </c>
+      <c r="G21" s="9"/>
       <c r="H21" s="2"/>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="3" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="D22" s="5">
-        <v>0.13084799999999999</v>
-      </c>
-      <c r="F22" s="3"/>
-      <c r="H22" s="2"/>
+        <v>92</v>
+      </c>
+      <c r="D22" s="6">
+        <v>0.70556700000000006</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D23" s="6">
+        <v>0.84280200000000005</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D24" s="6">
+        <v>0.69631100000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D25" s="6">
+        <v>8.5280999999999996E-2</v>
+      </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D25">
+    <sortCondition ref="A2:A25"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B9A0115-0DA3-4329-A43A-DAA03AB5F30D}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1130,7 +1224,7 @@
     <col min="4" max="4" width="9.85546875" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -1144,161 +1238,174 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:8">
       <c r="A2" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="5">
+        <v>0.57070699999999996</v>
+      </c>
+      <c r="H2" s="10"/>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" s="5">
+        <v>0.82667000000000002</v>
+      </c>
+      <c r="H3" s="10"/>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="5">
+        <v>0.98271600000000003</v>
+      </c>
+      <c r="H4" s="10"/>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D5" s="5">
         <v>0.91569699999999998</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="7" t="s">
+      <c r="H5" s="10"/>
+    </row>
+    <row r="6" spans="1:8" ht="30">
+      <c r="A6" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="5">
+        <v>0.99287499999999995</v>
+      </c>
+      <c r="H6" s="10"/>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="5">
+        <v>0.19645399999999999</v>
+      </c>
+      <c r="H7" s="10"/>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="5">
+        <v>0.62406399999999995</v>
+      </c>
+      <c r="H8" s="10"/>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D9" s="5">
         <v>0.345078</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="30">
-      <c r="A4" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="5">
-        <v>0.99287499999999995</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="5">
-        <v>0.98271600000000003</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="5">
-        <v>0.19645399999999999</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="5">
-        <v>0.62406399999999995</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" s="5">
-        <v>0.57070699999999996</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="7" t="s">
+      <c r="H9" s="10"/>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="5">
+        <v>0.31648700000000002</v>
+      </c>
+      <c r="H10" s="10"/>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B11" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D11" s="5">
         <v>0.999</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="7" t="s">
+      <c r="H11" s="10"/>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B12" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C12" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D12" s="5">
         <v>0.90539000000000003</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D11" s="5">
-        <v>0.82667000000000002</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D12" s="5">
-        <v>0.31648700000000002</v>
-      </c>
-    </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D12">
+    <sortCondition ref="A2:A12"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Data download script. Completed new estimation for philips curve
</commit_message>
<xml_diff>
--- a/Smets_Warne_Wouters_2014/Model_Inputs.xlsx
+++ b/Smets_Warne_Wouters_2014/Model_Inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\DSGE_Routledge\Smets_Warne_Wouters_2014\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17DBFD3E-DEE5-41FA-9419-66C5FC1446BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8436E4F1-C373-48BB-B0BE-3D9A9D57DB2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{66EF218B-DC11-4D6A-BEE5-8BD9D8BBF969}"/>
+    <workbookView xWindow="4815" yWindow="4185" windowWidth="21600" windowHeight="11295" xr2:uid="{66EF218B-DC11-4D6A-BEE5-8BD9D8BBF969}"/>
   </bookViews>
   <sheets>
     <sheet name="Parametry" sheetId="2" r:id="rId1"/>
@@ -785,8 +785,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BE39027-846B-4168-A1BF-4076619A79DB}">
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G7" sqref="G1:G1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>